<commit_message>
CP_MACDRSI.py eingefahren - output und Result konsolidiert Frist version of seasonal.py - Ausbau zum Lesen von Yahoo Daten mit Udemy Kurs Pandas
</commit_message>
<xml_diff>
--- a/input/Tickers - Kopie.xlsx
+++ b/input/Tickers - Kopie.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\System Development\IBKR\IAB API System\IAB API\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983933F3-3E01-4931-A675-9C9F382D9FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9207DEE4-6263-449F-9400-054D1EC190D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="100" windowWidth="35790" windowHeight="20050" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39300" yWindow="2620" windowWidth="23080" windowHeight="15450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tickers" sheetId="1" r:id="rId1"/>
     <sheet name="Index" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle1" sheetId="3" r:id="rId3"/>
-    <sheet name="TickTest" sheetId="4" r:id="rId4"/>
+    <sheet name="IVY11" sheetId="5" r:id="rId4"/>
+    <sheet name="TickTest" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2531" uniqueCount="1257">
   <si>
     <t>Company Name</t>
   </si>
@@ -3725,6 +3726,75 @@
   </si>
   <si>
     <t>IBKR</t>
+  </si>
+  <si>
+    <t>VNQ</t>
+  </si>
+  <si>
+    <t>Real Estate US</t>
+  </si>
+  <si>
+    <t>Real Estate ex-US</t>
+  </si>
+  <si>
+    <t>VNQI</t>
+  </si>
+  <si>
+    <t>Bonds US</t>
+  </si>
+  <si>
+    <t>BND</t>
+  </si>
+  <si>
+    <t>Bonds ex-US</t>
+  </si>
+  <si>
+    <t>BNDX</t>
+  </si>
+  <si>
+    <t>Energy Rohstoffe XLE besser</t>
+  </si>
+  <si>
+    <t>DBE</t>
+  </si>
+  <si>
+    <t>Edelmetalle</t>
+  </si>
+  <si>
+    <t>DBP</t>
+  </si>
+  <si>
+    <t>Industriemetalle</t>
+  </si>
+  <si>
+    <t>DBB</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>DBA</t>
+  </si>
+  <si>
+    <t>Emergingmarket</t>
+  </si>
+  <si>
+    <t>Stocks nonUS</t>
+  </si>
+  <si>
+    <t>Stocks US</t>
+  </si>
+  <si>
+    <t>VTI</t>
+  </si>
+  <si>
+    <t>Energieaktien Öl</t>
+  </si>
+  <si>
+    <t>Cash 1-3 y US-treasury</t>
+  </si>
+  <si>
+    <t>SHY</t>
   </si>
 </sst>
 </file>
@@ -4566,7 +4636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4577,7 +4647,7 @@
   <dimension ref="A1:D600"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -13232,10 +13302,224 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1073DA19-C5B0-48EC-9052-C8EB2C73CFC2}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="24.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B10" t="s">
+        <v>601</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B11" t="s">
+        <v>599</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B13" t="s">
+        <v>943</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084B43D0-4C61-417F-93AA-FE23E078E38E}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>